<commit_message>
Se arregló el error con horarios sin vacantes
</commit_message>
<xml_diff>
--- a/buffer.xlsx
+++ b/buffer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,20 +466,10 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Salón</t>
+          <t>Cupo</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Cupo</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Vacantes</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Nombre</t>
         </is>
@@ -487,14 +477,14 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1867</v>
+        <v>1052</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>M.I. JOSE ANTONIO DE JESUS ARREDONDO GARZA  (PRESENCIAL)</t>
+          <t>LIC. MARTHA MANCILLA URREA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -504,7 +494,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10:00 a 11:30</t>
+          <t>11:00 a 13:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -512,33 +502,25 @@
           <t>Lun, Mie</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>B106</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>35</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+      <c r="G2" t="n">
+        <v>37</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1867</v>
+        <v>1052</v>
       </c>
       <c r="B3" t="n">
         <v>2</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>M.I. PEDRO IGNACIO RINCON GOMEZ  (PRESENCIAL)</t>
+          <t>LIC ALDO FERNANDO TRUJILLO PRIEGO  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -548,7 +530,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>19:00 a 20:30</t>
+          <t>11:00 a 13:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -556,33 +538,25 @@
           <t>Lun, Mie</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Y001</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>35</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+      <c r="G3" t="n">
+        <v>37</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1867</v>
+        <v>1052</v>
       </c>
       <c r="B4" t="n">
         <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ING. JULIO CESAR CRUZ ESTRADA  (PRESENCIAL)</t>
+          <t>MTRA ANA LUISA SELENE ALVAREZ CARRILLO  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -592,41 +566,33 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>07:00 a 08:30</t>
+          <t>13:00 a 15:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Mar, Jue</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>J110</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>35</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+          <t>Lun, Mie</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>37</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1867</v>
+        <v>1052</v>
       </c>
       <c r="B5" t="n">
         <v>4</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ING. CARLOS SAUCEDO MACIEL  (PRESENCIAL)</t>
+          <t>LIC. MARTHA MANCILLA URREA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -636,41 +602,33 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>10:00 a 13:00</t>
+          <t>13:00 a 15:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Sab</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>J110</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>35</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+          <t>Lun, Mie</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>37</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1867</v>
+        <v>1052</v>
       </c>
       <c r="B6" t="n">
         <v>5</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>M.I. JOSE LUIS CRUZ MORA  (PRESENCIAL)</t>
+          <t>MTRA. AMELIA GUADALUPE FIEL RIVERA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -680,134 +638,110 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>10:00 a 13:00</t>
+          <t>17:00 a 19:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Sab</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>B204</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>35</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+          <t>Lun, Mie</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>37</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6867</v>
+        <v>1052</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ING. ROSA ELENA LOBERA SANCHEZ  (PRESENCIAL)</t>
+          <t>LIC. MARTHA MANCILLA URREA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>L+</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>07:00 a 09:00</t>
+          <t>17:00 a 19:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Mar</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Q209</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>22</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+          <t>Lun, Mie</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>37</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6867</v>
+        <v>1052</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>M.I. LUIS SERGIO DURAN ARENAS  (PRESENCIAL)</t>
+          <t>DR. ROGELIO DEL PRADO FLORES  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>L+</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>15:00 a 17:00</t>
+          <t>19:00 a 21:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Mar</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Q209</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>22</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+          <t>Lun, Mie</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>37</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6867</v>
+        <v>1052</v>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ING. ROSA ELENA LOBERA SANCHEZ  (PRESENCIAL)</t>
+          <t>DR. RAFAEL IRIARTE VIVAR-BALDERRAMA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>L+</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -817,256 +751,208 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Mie</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Q209</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>22</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>37</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>6867</v>
+        <v>1052</v>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>M.I. PEDRO IGNACIO RINCON GOMEZ  (PRESENCIAL)</t>
+          <t>LIC. MARIA DE GUADALUPE FLOR DIAZ DE LEON FERNANDEZ DE CASTRO  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>L+</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>17:00 a 19:00</t>
+          <t>09:00 a 11:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Mie</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Q209</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>22</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>37</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>6867</v>
+        <v>1052</v>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>M.I. LUIS SERGIO DURAN ARENAS  (PRESENCIAL)</t>
+          <t>MES. MARGARITA PUEBLA CADENA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>L+</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>17:00 a 19:00</t>
+          <t>11:00 a 13:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Jue</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Q209</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>22</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>37</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>6867</v>
+        <v>1052</v>
       </c>
       <c r="B12" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ING. JULIO CESAR CRUZ ESTRADA  (PRESENCIAL)</t>
+          <t>LIC ALDO FERNANDO TRUJILLO PRIEGO  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>L+</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>07:00 a 09:00</t>
+          <t>13:00 a 15:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Vie</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Q209</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>22</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>37</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>6867</v>
+        <v>1052</v>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>M.A. AYESHA SAGRARIO ROMAN GARCIA  (PRESENCIAL)</t>
+          <t>LIC. OCTAVIO EDUARDO VIZCAYA XILOTL  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>L+</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>20:00 a 22:00</t>
+          <t>15:00 a 17:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Vie</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Q209</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>22</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>37</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>6867</v>
+        <v>1052</v>
       </c>
       <c r="B14" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MTRO. JORGE FERAT TOSCANO  (PRESENCIAL)</t>
+          <t>DRA. OLINCA SUAREZ MEJIA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>L+</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>07:00 a 09:00</t>
+          <t>17:00 a 19:00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Sab</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Q209</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>22</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>37</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1858</v>
+        <v>1052</v>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ING. SAMUEL GANDARILLA PEREZ  (PRESENCIAL)</t>
+          <t>LIC. OCTAVIO EDUARDO VIZCAYA XILOTL  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1076,85 +962,69 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>11:30 a 13:00</t>
+          <t>17:00 a 19:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Mie, Vie</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>B305</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>35</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>SISTEMAS EMBEBIDOS</t>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>37</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1858</v>
+        <v>1052</v>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ING. SAMUEL GANDARILLA PEREZ  (PRESENCIAL)</t>
+          <t>M.I RENE ALVAREZ GUTIERREZ  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>11:00 a 13:00</t>
+          <t>19:00 a 21:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Lun</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>T101</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>35</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>SISTEMAS EMBEBIDOS</t>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>37</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1858</v>
+        <v>1052</v>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>M.C. JOSE MAURICIO MATAMOROS DE MARIA Y CAMPOS  (PRESENCIAL)</t>
+          <t>LIC. HUGO ULISES CRUZ (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1164,85 +1034,69 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>13:00 a 14:30</t>
+          <t>19:00 a 21:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Lun, Mie</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>B408</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>36</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>SISTEMAS EMBEBIDOS</t>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>37</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1858</v>
+        <v>1052</v>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>M.C. JOSE MAURICIO MATAMOROS DE MARIA Y CAMPOS  (PRESENCIAL)</t>
+          <t>LIC. ANGELA RENATA GOMEZ GONZALEZ  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>13:00 a 15:00</t>
+          <t>09:00 a 11:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Mar</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>P003</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>36</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>SISTEMAS EMBEBIDOS</t>
+          <t>Mie, Vie</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>37</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1858</v>
+        <v>1052</v>
       </c>
       <c r="B19" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>M.C. GERARDO ARIEL CASTILLO GARCIA  (PRESENCIAL) (* Ver "Nota de Inglés")</t>
+          <t>LIC. ANGELA RENATA GOMEZ GONZALEZ  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1252,85 +1106,69 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>14:30 a 16:00</t>
+          <t>11:00 a 13:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Mar, Jue</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>A301</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>35</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>SISTEMAS EMBEBIDOS</t>
+          <t>Mie, Vie</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>37</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1858</v>
+        <v>1052</v>
       </c>
       <c r="B20" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>M.C. GERARDO ARIEL CASTILLO GARCIA  (PRESENCIAL) (* Ver "Nota de Inglés")</t>
+          <t>LIC. ANGELA RENATA GOMEZ GONZALEZ  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>13:00 a 15:00</t>
+          <t>15:00 a 17:00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Lun</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>T101</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>35</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>SISTEMAS EMBEBIDOS</t>
+          <t>Mie, Vie</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>37</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1858</v>
+        <v>1052</v>
       </c>
       <c r="B21" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ING. SAMUEL GANDARILLA PEREZ  (PRESENCIAL)</t>
+          <t>LIC. ANGELA RENATA GOMEZ GONZALEZ  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1340,7 +1178,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>17:00 a 18:30</t>
+          <t>17:00 a 19:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1348,77 +1186,61 @@
           <t>Mie, Vie</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>B106</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>36</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>SISTEMAS EMBEBIDOS</t>
+      <c r="G21" t="n">
+        <v>37</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1858</v>
+        <v>1052</v>
       </c>
       <c r="B22" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ING. SAMUEL GANDARILLA PEREZ  (PRESENCIAL)</t>
+          <t>MTRO ENRIQUE OCTAVIO DIAZ CERON  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>17:00 a 19:00</t>
+          <t>09:00 a 13:00</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Lun</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>T101</t>
-        </is>
-      </c>
-      <c r="H22" t="n">
-        <v>36</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>SISTEMAS EMBEBIDOS</t>
+          <t>Vie</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>37</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1858</v>
+        <v>1052</v>
       </c>
       <c r="B23" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>M.A. AYESHA SAGRARIO ROMAN GARCIA  (PRESENCIAL)</t>
+          <t>DRA. OLINCA SUAREZ MEJIA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1428,51 +1250,43 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>19:00 a 20:30</t>
+          <t>13:00 a 17:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Mar, Jue</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>B206</t>
-        </is>
-      </c>
-      <c r="H23" t="n">
-        <v>36</v>
-      </c>
-      <c r="I23" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>SISTEMAS EMBEBIDOS</t>
+          <t>Vie</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>37</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1858</v>
+        <v>1052</v>
       </c>
       <c r="B24" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>M.A. AYESHA SAGRARIO ROMAN GARCIA  (PRESENCIAL)</t>
+          <t>LIC. RICARDO TRÁNSITO SANTOS  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>18:00 a 20:00</t>
+          <t>15:00 a 19:00</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1480,33 +1294,25 @@
           <t>Vie</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Q209</t>
-        </is>
-      </c>
-      <c r="H24" t="n">
-        <v>36</v>
-      </c>
-      <c r="I24" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>SISTEMAS EMBEBIDOS</t>
+      <c r="G24" t="n">
+        <v>37</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1959</v>
+        <v>1052</v>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>M.I. JOSE ANTONIO AYALA BARBOSA  (PRESENCIAL)</t>
+          <t>DRA. OLINCA SUAREZ MEJIA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1516,41 +1322,33 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>07:00 a 09:00</t>
+          <t>08:00 a 12:00</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Lun, Mie</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>B204</t>
-        </is>
-      </c>
-      <c r="H25" t="n">
-        <v>40</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>SISTEMAS DISTRIBUIDOS</t>
+          <t>Sab</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>37</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1959</v>
+        <v>1052</v>
       </c>
       <c r="B26" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>M.I. ELBA KAREN SAENZ GARCIA  (PRESENCIAL)</t>
+          <t>MTRA NORMA ANGELICA OCAMPO MENDOZA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1560,41 +1358,33 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>11:00 a 13:00</t>
+          <t>17:00 a 19:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Lun, Vie</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>J111</t>
-        </is>
-      </c>
-      <c r="H26" t="n">
-        <v>40</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>SISTEMAS DISTRIBUIDOS</t>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>37</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>ETICA PROFESIONAL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1959</v>
+        <v>1867</v>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>LIC. ARMANDO REYES GALICIA  (PRESENCIAL)</t>
+          <t>M.I. JOSE ANTONIO DE JESUS ARREDONDO GARZA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1604,41 +1394,33 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>09:00 a 11:00</t>
+          <t>10:00 a 11:30</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Mar, Jue</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>B206</t>
-        </is>
-      </c>
-      <c r="H27" t="n">
-        <v>40</v>
-      </c>
-      <c r="I27" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>SISTEMAS DISTRIBUIDOS</t>
+          <t>Lun, Mie</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>35</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1959</v>
+        <v>1867</v>
       </c>
       <c r="B28" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ING. JOSE ABRAHAM BONILLA PASTOR  (PRESENCIAL)</t>
+          <t>M.I. PEDRO IGNACIO RINCON GOMEZ  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1648,41 +1430,33 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>19:00 a 21:00</t>
+          <t>19:00 a 20:30</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Mar, Jue</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>B305</t>
-        </is>
-      </c>
-      <c r="H28" t="n">
-        <v>40</v>
-      </c>
-      <c r="I28" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>SISTEMAS DISTRIBUIDOS</t>
+          <t>Lun, Mie</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>35</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1959</v>
+        <v>1867</v>
       </c>
       <c r="B29" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ING. GUADALUPE LIZETH PARRALES ROMAY  (PRESENCIAL)</t>
+          <t>ING. JULIO CESAR CRUZ ESTRADA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1692,41 +1466,33 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>09:00 a 13:00</t>
+          <t>07:00 a 08:30</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Sab</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>A206</t>
-        </is>
-      </c>
-      <c r="H29" t="n">
-        <v>40</v>
-      </c>
-      <c r="I29" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>SISTEMAS DISTRIBUIDOS</t>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>35</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2928</v>
+        <v>1867</v>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ING. JULIO ALFONSO DE LEON RAZO  (PRESENCIAL)</t>
+          <t>ING. CARLOS SAUCEDO MACIEL  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1736,41 +1502,33 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>19:00 a 21:00</t>
+          <t>10:00 a 13:00</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Lun, Mie</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>A302</t>
-        </is>
-      </c>
-      <c r="H30" t="n">
-        <v>40</v>
-      </c>
-      <c r="I30" t="n">
-        <v>0</v>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>ADMINISTRACION PROYECTOS TIC</t>
+          <t>Sab</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>35</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2928</v>
+        <v>1867</v>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ING. JONATHAN GAMBOA BELTRAN  (PRESENCIAL) (* Ver "Nota de Inglés")</t>
+          <t>M.I. JOSE LUIS CRUZ MORA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1780,95 +1538,79 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>07:00 a 09:00</t>
+          <t>10:00 a 13:00</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Mar, Jue</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>D004</t>
-        </is>
-      </c>
-      <c r="H31" t="n">
-        <v>40</v>
-      </c>
-      <c r="I31" t="n">
-        <v>0</v>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>ADMINISTRACION PROYECTOS TIC</t>
+          <t>Sab</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>35</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2958</v>
+        <v>6867</v>
       </c>
       <c r="B32" t="n">
         <v>1</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ING. ARTURO PEREZ DE LA CRUZ  (PRESENCIAL)</t>
+          <t>ING. ROSA ELENA LOBERA SANCHEZ  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>L+</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>13:00 a 15:00</t>
+          <t>07:00 a 09:00</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Lun, Mie</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Q218</t>
-        </is>
-      </c>
-      <c r="H32" t="n">
-        <v>15</v>
-      </c>
-      <c r="I32" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>TEMAS SELECTOS INGENIERIA COMPUTACION III</t>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>22</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>2958</v>
+        <v>6867</v>
       </c>
       <c r="B33" t="n">
         <v>2</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>M.I. JOSE ANTONIO MACIAS GARCIA  (PRESENCIAL)</t>
+          <t>M.I. LUIS SERGIO DURAN ARENAS  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>L+</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>13:00 a 15:00</t>
+          <t>15:00 a 17:00</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1876,64 +1618,840 @@
           <t>Mar</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Y002</t>
-        </is>
-      </c>
-      <c r="H33" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" t="n">
-        <v>0</v>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>TEMAS SELECTOS INGENIERIA COMPUTACION III</t>
+      <c r="G33" t="n">
+        <v>22</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>2958</v>
+        <v>6867</v>
       </c>
       <c r="B34" t="n">
+        <v>3</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ING. ROSA ELENA LOBERA SANCHEZ  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>L+</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>07:00 a 09:00</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Mie</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>22</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>6867</v>
+      </c>
+      <c r="B35" t="n">
+        <v>4</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>M.I. PEDRO IGNACIO RINCON GOMEZ  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>L+</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>17:00 a 19:00</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Mie</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>22</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>6867</v>
+      </c>
+      <c r="B36" t="n">
+        <v>5</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>M.I. LUIS SERGIO DURAN ARENAS  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>L+</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>17:00 a 19:00</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Jue</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>22</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>6867</v>
+      </c>
+      <c r="B37" t="n">
+        <v>6</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ING. JULIO CESAR CRUZ ESTRADA  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>L+</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>07:00 a 09:00</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Vie</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>22</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>6867</v>
+      </c>
+      <c r="B38" t="n">
+        <v>7</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>M.A. AYESHA SAGRARIO ROMAN GARCIA  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>L+</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>20:00 a 22:00</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Vie</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>22</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>6867</v>
+      </c>
+      <c r="B39" t="n">
+        <v>8</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>MTRO. JORGE FERAT TOSCANO  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>L+</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>07:00 a 09:00</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Sab</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>22</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>L.ORGANIZACION ARQUITECTURA COMPUTADORAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1858</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>ING. SAMUEL GANDARILLA PEREZ  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>11:30 a 13:00</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Mie, Vie</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>35</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>EMBEBIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1858</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>ING. SAMUEL GANDARILLA PEREZ  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>11:00 a 13:00</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Lun</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>35</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>EMBEBIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1858</v>
+      </c>
+      <c r="B42" t="n">
         <v>2</v>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>M.I. JOSE ANTONIO MACIAS GARCIA  (PRESENCIAL)</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>T</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>M.C. JOSE MAURICIO MATAMOROS DE MARIA Y CAMPOS  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>13:00 a 14:30</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Lun, Mie</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>35</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>EMBEBIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1858</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>M.C. JOSE MAURICIO MATAMOROS DE MARIA Y CAMPOS  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
         <is>
           <t>13:00 a 15:00</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Jue</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Q208</t>
-        </is>
-      </c>
-      <c r="H34" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" t="n">
-        <v>0</v>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>TEMAS SELECTOS INGENIERIA COMPUTACION III</t>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>35</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>EMBEBIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1858</v>
+      </c>
+      <c r="B44" t="n">
+        <v>3</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>M.C. GERARDO ARIEL CASTILLO GARCIA  (PRESENCIAL) (* Ver "Nota de Inglés")</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>14:30 a 16:00</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>35</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>EMBEBIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1858</v>
+      </c>
+      <c r="B45" t="n">
+        <v>3</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>M.C. GERARDO ARIEL CASTILLO GARCIA  (PRESENCIAL) (* Ver "Nota de Inglés")</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>13:00 a 15:00</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Lun</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>35</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>EMBEBIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1858</v>
+      </c>
+      <c r="B46" t="n">
+        <v>4</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>ING. SAMUEL GANDARILLA PEREZ  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>17:00 a 18:30</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Mie, Vie</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>35</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>EMBEBIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1858</v>
+      </c>
+      <c r="B47" t="n">
+        <v>4</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>ING. SAMUEL GANDARILLA PEREZ  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>17:00 a 19:00</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Lun</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>35</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>EMBEBIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1858</v>
+      </c>
+      <c r="B48" t="n">
+        <v>5</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>M.A. AYESHA SAGRARIO ROMAN GARCIA  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>19:00 a 20:30</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>35</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>EMBEBIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1858</v>
+      </c>
+      <c r="B49" t="n">
+        <v>5</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>M.A. AYESHA SAGRARIO ROMAN GARCIA  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>18:00 a 20:00</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Vie</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>35</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>EMBEBIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>2948</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>ING. REYNALDO MARTELL AVILA  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>10:00 a 14:00</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Sab</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>30</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>COMPUTACION GRAFICA AVANZADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>2957</v>
+      </c>
+      <c r="B51" t="n">
+        <v>2</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>DR. SERGIO TEODORO VITE  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>15:00 a 16:30</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Lun, Mie</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>15</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>TEMAS SELECTOS INGENIERIA COMPUTACION II</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>2957</v>
+      </c>
+      <c r="B52" t="n">
+        <v>3</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>ING. EDUARDO DANIEL GUERRERO RAMIREZ  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>07:00 a 10:00</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Vie</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>15</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>TEMAS SELECTOS INGENIERIA COMPUTACION II</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>2957</v>
+      </c>
+      <c r="B53" t="n">
+        <v>4</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ING. VIRGINIA CECILIA DIAZ GARCIA  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>08:00 a 11:00</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Sab</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>15</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>TEMAS SELECTOS INGENIERIA COMPUTACION II</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>2957</v>
+      </c>
+      <c r="B54" t="n">
+        <v>5</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>ING. HEIDDY ALEJANDRA PASTEN LUGO  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>07:00 a 10:00</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Sab</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>15</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>TEMAS SELECTOS INGENIERIA COMPUTACION II</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>2928</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>ING. JULIO ALFONSO DE LEON RAZO  (PRESENCIAL)</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>19:00 a 21:00</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Lun, Mie</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>40</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>ADMINISTRACION PROYECTOS TIC</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>2928</v>
+      </c>
+      <c r="B56" t="n">
+        <v>2</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>ING. FRANCISCO XAVIER JIMAREZ RODRIGUEZ  (PRESENCIAL) (* Ver "Nota de Inglés")</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>15:00 a 17:00</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Mar, Jue</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>40</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>ADMINISTRACION PROYECTOS TIC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se añadio el codigo dinamico
</commit_message>
<xml_diff>
--- a/buffer.xlsx
+++ b/buffer.xlsx
@@ -2241,14 +2241,14 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>2957</v>
+        <v>2928</v>
       </c>
       <c r="B51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>DR. SERGIO TEODORO VITE  (PRESENCIAL)</t>
+          <t>ING. JULIO ALFONSO DE LEON RAZO  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>15:00 a 16:30</t>
+          <t>19:00 a 21:00</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2267,24 +2267,24 @@
         </is>
       </c>
       <c r="G51" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>TEMAS SELECTOS INGENIERIA COMPUTACION II</t>
+          <t>ADMINISTRACION PROYECTOS TIC</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2957</v>
+        <v>2928</v>
       </c>
       <c r="B52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ING. EDUARDO DANIEL GUERRERO RAMIREZ  (PRESENCIAL)</t>
+          <t>ING. FRANCISCO XAVIER JIMAREZ RODRIGUEZ  (PRESENCIAL) (* Ver "Nota de Inglés")</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2294,20 +2294,20 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>07:00 a 10:00</t>
+          <t>15:00 a 17:00</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Vie</t>
+          <t>Mar, Jue</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>TEMAS SELECTOS INGENIERIA COMPUTACION II</t>
+          <t>ADMINISTRACION PROYECTOS TIC</t>
         </is>
       </c>
     </row>
@@ -2316,11 +2316,11 @@
         <v>2957</v>
       </c>
       <c r="B53" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>ING. VIRGINIA CECILIA DIAZ GARCIA  (PRESENCIAL)</t>
+          <t>DR. SERGIO TEODORO VITE  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2330,12 +2330,12 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>08:00 a 11:00</t>
+          <t>15:00 a 16:30</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Sab</t>
+          <t>Lun, Mie</t>
         </is>
       </c>
       <c r="G53" t="n">
@@ -2352,11 +2352,11 @@
         <v>2957</v>
       </c>
       <c r="B54" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>ING. HEIDDY ALEJANDRA PASTEN LUGO  (PRESENCIAL)</t>
+          <t>ING. EDUARDO DANIEL GUERRERO RAMIREZ  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2371,7 +2371,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Sab</t>
+          <t>Vie</t>
         </is>
       </c>
       <c r="G54" t="n">
@@ -2385,14 +2385,14 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2928</v>
+        <v>2957</v>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>ING. JULIO ALFONSO DE LEON RAZO  (PRESENCIAL)</t>
+          <t>ING. VIRGINIA CECILIA DIAZ GARCIA  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2402,33 +2402,33 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>19:00 a 21:00</t>
+          <t>08:00 a 11:00</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Lun, Mie</t>
+          <t>Sab</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>ADMINISTRACION PROYECTOS TIC</t>
+          <t>TEMAS SELECTOS INGENIERIA COMPUTACION II</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2928</v>
+        <v>2957</v>
       </c>
       <c r="B56" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ING. FRANCISCO XAVIER JIMAREZ RODRIGUEZ  (PRESENCIAL) (* Ver "Nota de Inglés")</t>
+          <t>ING. HEIDDY ALEJANDRA PASTEN LUGO  (PRESENCIAL)</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2438,20 +2438,20 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>15:00 a 17:00</t>
+          <t>07:00 a 10:00</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Mar, Jue</t>
+          <t>Sab</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>ADMINISTRACION PROYECTOS TIC</t>
+          <t>TEMAS SELECTOS INGENIERIA COMPUTACION II</t>
         </is>
       </c>
     </row>

</xml_diff>